<commit_message>
removed address validation while hsphere user import
</commit_message>
<xml_diff>
--- a/deployments/users.xlsx
+++ b/deployments/users.xlsx
@@ -73,13 +73,13 @@
     <t>hsphere cluster id</t>
   </si>
   <si>
-    <t>Test 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> User 14</t>
-  </si>
-  <si>
-    <t>htest14@hspheretest.com</t>
+    <t>Test 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> User 20</t>
+  </si>
+  <si>
+    <t>htest20@hspheretest.com</t>
   </si>
   <si>
     <t>Syed@123</t>
@@ -97,7 +97,7 @@
     <t>UP</t>
   </si>
   <si>
-    <t>IN</t>
+    <t>US</t>
   </si>
   <si>
     <t>due</t>
@@ -106,13 +106,13 @@
     <t>monthly</t>
   </si>
   <si>
-    <t>Test 15</t>
-  </si>
-  <si>
-    <t>User 15</t>
-  </si>
-  <si>
-    <t>htest15@hspheretest.com</t>
+    <t>Test 21</t>
+  </si>
+  <si>
+    <t>User 21</t>
+  </si>
+  <si>
+    <t>htest21@hspheretest.com</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
       <c r="M2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="O2" s="3">
@@ -596,7 +596,7 @@
       <c r="M3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="O3" s="3">
@@ -615,7 +615,7 @@
         <v>30</v>
       </c>
       <c r="T3" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1"/>

</xml_diff>